<commit_message>
ci: add GitHub Actions workflow and CI-controlled test execution
</commit_message>
<xml_diff>
--- a/DemoData/TestPlan.xlsx
+++ b/DemoData/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sdet-framework-reference\DemoData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF9DE5-BABA-4751-8752-D1E0EF13A97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF72B0-D8F7-4FFA-9446-A9846AF6D77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5904" yWindow="0" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDir" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>TestName</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>add_item_to_cart</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>默認為index=0加入第一個商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>index=0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -234,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -248,6 +260,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +582,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -643,10 +658,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D653F17-7651-4C82-8B74-0BA06AE6A92F}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -654,12 +669,13 @@
     <col min="1" max="1" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.875" style="2"/>
-    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="36.875" style="2"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.875" style="2"/>
+    <col min="6" max="6" width="30.5" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="36.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -670,13 +686,16 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -686,11 +705,12 @@
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="3"/>
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -700,8 +720,9 @@
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -711,7 +732,13 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>